<commit_message>
Seleçao de casos para testage
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/Comparação entre número de pertubações.xlsx
+++ b/Arquivos/Comparações/Comparação entre número de pertubações.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12885"/>
+    <workbookView windowWidth="28110" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Comparações do ILS em relação ao número de pertubações</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>ulysses22</t>
+  </si>
+  <si>
+    <t>Número de vezes que cada caso foi melhor</t>
+  </si>
+  <si>
+    <t>Média dos resultados</t>
   </si>
 </sst>
 </file>
@@ -368,12 +374,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -738,146 +750,146 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -908,13 +920,31 @@
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1251,16 +1281,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:M49"/>
+  <dimension ref="B2:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="11.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="13.1619047619048" customWidth="1"/>
     <col min="4" max="6" width="13.2857142857143" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="13" width="17.8571428571429" customWidth="1"/>
@@ -1299,7 +1329,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="10"/>
+      <c r="L3" s="18"/>
       <c r="M3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1353,22 +1383,24 @@
         <v>1325</v>
       </c>
       <c r="G5" s="9">
-        <v>2631</v>
-      </c>
-      <c r="H5" s="9">
-        <v>2989</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1315</v>
-      </c>
-      <c r="J5" s="11">
         <v>1239</v>
       </c>
-      <c r="K5" s="11">
-        <v>1315</v>
-      </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="13">
+      <c r="H5" s="10">
+        <v>1325</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1239</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1604</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1239</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1239</v>
+      </c>
+      <c r="M5" s="19">
         <f>SMALL(D5:L5,1)</f>
         <v>1239</v>
       </c>
@@ -1390,22 +1422,24 @@
         <v>268</v>
       </c>
       <c r="G6" s="9">
-        <v>306</v>
-      </c>
-      <c r="H6" s="9">
-        <v>306</v>
-      </c>
-      <c r="I6" s="11">
-        <v>275</v>
-      </c>
-      <c r="J6" s="11">
-        <v>275</v>
-      </c>
-      <c r="K6" s="11">
-        <v>275</v>
-      </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13">
+        <v>274</v>
+      </c>
+      <c r="H6" s="10">
+        <v>246</v>
+      </c>
+      <c r="I6" s="9">
+        <v>268</v>
+      </c>
+      <c r="J6" s="9">
+        <v>246</v>
+      </c>
+      <c r="K6" s="9">
+        <v>274</v>
+      </c>
+      <c r="L6" s="9">
+        <v>246</v>
+      </c>
+      <c r="M6" s="19">
         <f>SMALL(D6:L6,1)</f>
         <v>246</v>
       </c>
@@ -1427,22 +1461,24 @@
         <v>282</v>
       </c>
       <c r="G7" s="9">
-        <v>338</v>
-      </c>
-      <c r="H7" s="9">
-        <v>341</v>
-      </c>
-      <c r="I7" s="11">
+        <v>331</v>
+      </c>
+      <c r="H7" s="10">
+        <v>382</v>
+      </c>
+      <c r="I7" s="9">
+        <v>331</v>
+      </c>
+      <c r="J7" s="9">
+        <v>510</v>
+      </c>
+      <c r="K7" s="9">
+        <v>282</v>
+      </c>
+      <c r="L7" s="9">
         <v>319</v>
       </c>
-      <c r="J7" s="11">
-        <v>319</v>
-      </c>
-      <c r="K7" s="11">
-        <v>319</v>
-      </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="13">
+      <c r="M7" s="19">
         <f>SMALL(D7:L7,1)</f>
         <v>282</v>
       </c>
@@ -1464,22 +1500,24 @@
         <v>480.48</v>
       </c>
       <c r="G8" s="9">
-        <v>503.52</v>
-      </c>
-      <c r="H8" s="9">
-        <v>503.52</v>
-      </c>
-      <c r="I8" s="11">
-        <v>556.81</v>
-      </c>
-      <c r="J8" s="11">
         <v>480.48</v>
       </c>
-      <c r="K8" s="11">
-        <v>556.81</v>
-      </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="13">
+      <c r="H8" s="10">
+        <v>480.48</v>
+      </c>
+      <c r="I8" s="9">
+        <v>480.48</v>
+      </c>
+      <c r="J8" s="9">
+        <v>480.48</v>
+      </c>
+      <c r="K8" s="9">
+        <v>480.48</v>
+      </c>
+      <c r="L8" s="9">
+        <v>480.48</v>
+      </c>
+      <c r="M8" s="19">
         <f>SMALL(D8:L8,1)</f>
         <v>480.48</v>
       </c>
@@ -1501,24 +1539,26 @@
         <v>14206.79</v>
       </c>
       <c r="G9" s="9">
-        <v>12394.2</v>
-      </c>
-      <c r="H9" s="9">
-        <v>15151.08</v>
-      </c>
-      <c r="I9" s="11">
-        <v>13213.67</v>
-      </c>
-      <c r="J9" s="11">
-        <v>13213.67</v>
-      </c>
-      <c r="K9" s="11">
-        <v>13213.67</v>
-      </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="13">
+        <v>13734.2</v>
+      </c>
+      <c r="H9" s="10">
+        <v>14078.75</v>
+      </c>
+      <c r="I9" s="9">
+        <v>15747.31</v>
+      </c>
+      <c r="J9" s="9">
+        <v>13434.51</v>
+      </c>
+      <c r="K9" s="9">
+        <v>14993.24</v>
+      </c>
+      <c r="L9" s="9">
+        <v>13481.44</v>
+      </c>
+      <c r="M9" s="19">
         <f>SMALL(D9:L9,1)</f>
-        <v>12394.2</v>
+        <v>13434.51</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="2:13">
@@ -1538,24 +1578,26 @@
         <v>3891</v>
       </c>
       <c r="G10" s="9">
-        <v>3795</v>
-      </c>
-      <c r="H10" s="9">
-        <v>3851</v>
-      </c>
-      <c r="I10" s="11">
-        <v>4077</v>
-      </c>
-      <c r="J10" s="11">
-        <v>4077</v>
-      </c>
-      <c r="K10" s="11">
-        <v>4077</v>
-      </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="13">
+        <v>4176</v>
+      </c>
+      <c r="H10" s="10">
+        <v>3908</v>
+      </c>
+      <c r="I10" s="9">
+        <v>4172</v>
+      </c>
+      <c r="J10" s="9">
+        <v>3087</v>
+      </c>
+      <c r="K10" s="9">
+        <v>3964</v>
+      </c>
+      <c r="L10" s="9">
+        <v>3766</v>
+      </c>
+      <c r="M10" s="19">
         <f>SMALL(D10:L10,1)</f>
-        <v>3795</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:13">
@@ -1575,24 +1617,26 @@
         <v>630</v>
       </c>
       <c r="G11" s="9">
+        <v>650</v>
+      </c>
+      <c r="H11" s="10">
+        <v>4090</v>
+      </c>
+      <c r="I11" s="9">
         <v>680</v>
       </c>
-      <c r="H11" s="9">
-        <v>600</v>
-      </c>
-      <c r="I11" s="11">
-        <v>470</v>
-      </c>
-      <c r="J11" s="11">
-        <v>470</v>
-      </c>
-      <c r="K11" s="11">
-        <v>470</v>
-      </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="13">
+      <c r="J11" s="9">
+        <v>720</v>
+      </c>
+      <c r="K11" s="9">
+        <v>730</v>
+      </c>
+      <c r="L11" s="9">
+        <v>720</v>
+      </c>
+      <c r="M11" s="19">
         <f>SMALL(D11:L11,1)</f>
-        <v>470</v>
+        <v>630</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="2:13">
@@ -1614,20 +1658,22 @@
       <c r="G12" s="9">
         <v>224.88</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="10">
         <v>224.88</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="9">
         <v>224.88</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="9">
         <v>224.88</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="9">
         <v>224.88</v>
       </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="13">
+      <c r="L12" s="9">
+        <v>224.88</v>
+      </c>
+      <c r="M12" s="19">
         <f>SMALL(D12:L12,1)</f>
         <v>224.88</v>
       </c>
@@ -1649,24 +1695,26 @@
         <v>1207.48</v>
       </c>
       <c r="G13" s="9">
-        <v>1501.67</v>
-      </c>
-      <c r="H13" s="9">
-        <v>1645.54</v>
-      </c>
-      <c r="I13" s="11">
-        <v>1171.54</v>
-      </c>
-      <c r="J13" s="11">
-        <v>1171.54</v>
-      </c>
-      <c r="K13" s="11">
-        <v>1171.54</v>
-      </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="13">
+        <v>1159.8</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1302.6</v>
+      </c>
+      <c r="I13" s="9">
+        <v>1277.39</v>
+      </c>
+      <c r="J13" s="9">
+        <v>1220.78</v>
+      </c>
+      <c r="K13" s="9">
+        <v>1883.32</v>
+      </c>
+      <c r="L13" s="9">
+        <v>1187.01</v>
+      </c>
+      <c r="M13" s="19">
         <f>SMALL(D13:L13,1)</f>
-        <v>1171.54</v>
+        <v>1159.8</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="2:13">
@@ -1686,24 +1734,26 @@
         <v>1414.89</v>
       </c>
       <c r="G14" s="9">
-        <v>1814.28</v>
-      </c>
-      <c r="H14" s="9">
-        <v>1848.76</v>
-      </c>
-      <c r="I14" s="11">
-        <v>1284.47</v>
-      </c>
-      <c r="J14" s="11">
-        <v>1284.47</v>
-      </c>
-      <c r="K14" s="11">
-        <v>1284.47</v>
-      </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="13">
+        <v>1676.07</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1394.95</v>
+      </c>
+      <c r="I14" s="9">
+        <v>1410.54</v>
+      </c>
+      <c r="J14" s="9">
+        <v>1304.99</v>
+      </c>
+      <c r="K14" s="9">
+        <v>1782</v>
+      </c>
+      <c r="L14" s="9">
+        <v>1711.8</v>
+      </c>
+      <c r="M14" s="19">
         <f>SMALL(D14:L14,1)</f>
-        <v>1284.47</v>
+        <v>1304.99</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="2:13">
@@ -1723,24 +1773,26 @@
         <v>120</v>
       </c>
       <c r="G15" s="9">
-        <v>176</v>
-      </c>
-      <c r="H15" s="9">
-        <v>138</v>
-      </c>
-      <c r="I15" s="11">
-        <v>99</v>
-      </c>
-      <c r="J15" s="11">
-        <v>99</v>
-      </c>
-      <c r="K15" s="11">
-        <v>99</v>
-      </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="13">
+        <v>98</v>
+      </c>
+      <c r="H15" s="10">
+        <v>136</v>
+      </c>
+      <c r="I15" s="9">
+        <v>113</v>
+      </c>
+      <c r="J15" s="9">
+        <v>163</v>
+      </c>
+      <c r="K15" s="9">
+        <v>111</v>
+      </c>
+      <c r="L15" s="9">
+        <v>108</v>
+      </c>
+      <c r="M15" s="19">
         <f>SMALL(D15:L15,1)</f>
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="2:13">
@@ -1760,24 +1812,26 @@
         <v>99.04</v>
       </c>
       <c r="G16" s="9">
-        <v>107.97</v>
-      </c>
-      <c r="H16" s="9">
-        <v>126.7</v>
-      </c>
-      <c r="I16" s="11">
-        <v>97.21</v>
-      </c>
-      <c r="J16" s="11">
-        <v>97.21</v>
-      </c>
-      <c r="K16" s="11">
-        <v>97.21</v>
-      </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="13">
+        <v>95.96</v>
+      </c>
+      <c r="H16" s="10">
+        <v>106.06</v>
+      </c>
+      <c r="I16" s="9">
+        <v>101.11</v>
+      </c>
+      <c r="J16" s="9">
+        <v>101.63</v>
+      </c>
+      <c r="K16" s="9">
+        <v>102.6</v>
+      </c>
+      <c r="L16" s="9">
+        <v>95.66</v>
+      </c>
+      <c r="M16" s="19">
         <f>SMALL(D16:L16,1)</f>
-        <v>95.88</v>
+        <v>95.66</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="2:13">
@@ -1797,22 +1851,24 @@
         <v>113.91</v>
       </c>
       <c r="G17" s="9">
-        <v>111.43</v>
-      </c>
-      <c r="H17" s="9">
-        <v>118.33</v>
-      </c>
-      <c r="I17" s="11">
-        <v>129.13</v>
-      </c>
-      <c r="J17" s="11">
-        <v>129.13</v>
-      </c>
-      <c r="K17" s="11">
-        <v>129.13</v>
-      </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="13">
+        <v>99.42</v>
+      </c>
+      <c r="H17" s="10">
+        <v>97.66</v>
+      </c>
+      <c r="I17" s="9">
+        <v>110.9</v>
+      </c>
+      <c r="J17" s="9">
+        <v>118.77</v>
+      </c>
+      <c r="K17" s="9">
+        <v>96.77</v>
+      </c>
+      <c r="L17" s="9">
+        <v>95.57</v>
+      </c>
+      <c r="M17" s="19">
         <f>SMALL(D17:L17,1)</f>
         <v>95.07</v>
       </c>
@@ -1834,22 +1890,24 @@
         <v>204</v>
       </c>
       <c r="G18" s="9">
-        <v>157</v>
-      </c>
-      <c r="H18" s="9">
-        <v>214</v>
-      </c>
-      <c r="I18" s="12">
         <v>145</v>
       </c>
-      <c r="J18" s="12">
+      <c r="H18" s="10">
         <v>145</v>
       </c>
-      <c r="K18" s="12">
+      <c r="I18" s="9">
         <v>145</v>
       </c>
-      <c r="L18" s="12"/>
-      <c r="M18" s="13">
+      <c r="J18" s="9">
+        <v>188</v>
+      </c>
+      <c r="K18" s="9">
+        <v>190</v>
+      </c>
+      <c r="L18" s="9">
+        <v>197</v>
+      </c>
+      <c r="M18" s="19">
         <f>SMALL(D18:L18,1)</f>
         <v>145</v>
       </c>
@@ -1871,22 +1929,24 @@
         <v>143</v>
       </c>
       <c r="G19" s="9">
+        <v>143</v>
+      </c>
+      <c r="H19" s="10">
+        <v>143</v>
+      </c>
+      <c r="I19" s="9">
+        <v>143</v>
+      </c>
+      <c r="J19" s="9">
         <v>154</v>
       </c>
-      <c r="H19" s="9">
+      <c r="K19" s="9">
         <v>143</v>
       </c>
-      <c r="I19" s="11">
+      <c r="L19" s="9">
         <v>143</v>
       </c>
-      <c r="J19" s="11">
-        <v>143</v>
-      </c>
-      <c r="K19" s="11">
-        <v>143</v>
-      </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="13">
+      <c r="M19" s="19">
         <f t="shared" ref="M19:M34" si="0">SMALL(D19:L19,1)</f>
         <v>143</v>
       </c>
@@ -1910,20 +1970,22 @@
       <c r="G20" s="9">
         <v>181</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="10">
         <v>181</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="9">
         <v>181</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="9">
         <v>181</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="9">
         <v>181</v>
       </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="13">
+      <c r="L20" s="9">
+        <v>181</v>
+      </c>
+      <c r="M20" s="19">
         <f t="shared" si="0"/>
         <v>181</v>
       </c>
@@ -1945,22 +2007,24 @@
         <v>162</v>
       </c>
       <c r="G21" s="9">
-        <v>305</v>
-      </c>
-      <c r="H21" s="9">
         <v>189</v>
       </c>
-      <c r="I21" s="11">
+      <c r="H21" s="10">
+        <v>189</v>
+      </c>
+      <c r="I21" s="9">
         <v>162</v>
       </c>
-      <c r="J21" s="11">
-        <v>162</v>
-      </c>
-      <c r="K21" s="11">
-        <v>162</v>
-      </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="13">
+      <c r="J21" s="9">
+        <v>189</v>
+      </c>
+      <c r="K21" s="9">
+        <v>189</v>
+      </c>
+      <c r="L21" s="9">
+        <v>189</v>
+      </c>
+      <c r="M21" s="19">
         <f t="shared" si="0"/>
         <v>162</v>
       </c>
@@ -1982,22 +2046,24 @@
         <v>788</v>
       </c>
       <c r="G22" s="9">
-        <v>1521</v>
-      </c>
-      <c r="H22" s="9">
-        <v>762</v>
-      </c>
-      <c r="I22" s="11">
-        <v>668</v>
-      </c>
-      <c r="J22" s="11">
-        <v>668</v>
-      </c>
-      <c r="K22" s="11">
-        <v>668</v>
-      </c>
-      <c r="L22" s="12"/>
-      <c r="M22" s="13">
+        <v>558</v>
+      </c>
+      <c r="H22" s="10">
+        <v>660</v>
+      </c>
+      <c r="I22" s="9">
+        <v>558</v>
+      </c>
+      <c r="J22" s="9">
+        <v>558</v>
+      </c>
+      <c r="K22" s="9">
+        <v>558</v>
+      </c>
+      <c r="L22" s="9">
+        <v>558</v>
+      </c>
+      <c r="M22" s="19">
         <f t="shared" si="0"/>
         <v>558</v>
       </c>
@@ -2019,24 +2085,26 @@
         <v>14201.73</v>
       </c>
       <c r="G23" s="9">
-        <v>15913.2</v>
-      </c>
-      <c r="H23" s="9">
-        <v>17874.94</v>
-      </c>
-      <c r="I23" s="11">
-        <v>9332.77</v>
-      </c>
-      <c r="J23" s="11">
-        <v>9332.77</v>
-      </c>
-      <c r="K23" s="11">
-        <v>9332.77</v>
-      </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="13">
+        <v>13696.3</v>
+      </c>
+      <c r="H23" s="10">
+        <v>15283.5</v>
+      </c>
+      <c r="I23" s="9">
+        <v>16104.96</v>
+      </c>
+      <c r="J23" s="9">
+        <v>12489.67</v>
+      </c>
+      <c r="K23" s="9">
+        <v>15012.24</v>
+      </c>
+      <c r="L23" s="9">
+        <v>19320.67</v>
+      </c>
+      <c r="M23" s="19">
         <f t="shared" si="0"/>
-        <v>9332.77</v>
+        <v>10729.18</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="2:13">
@@ -2056,24 +2124,26 @@
         <v>1255</v>
       </c>
       <c r="G24" s="9">
-        <v>1764</v>
-      </c>
-      <c r="H24" s="9">
-        <v>1694</v>
-      </c>
-      <c r="I24" s="11">
-        <v>1355</v>
-      </c>
-      <c r="J24" s="11">
-        <v>1355</v>
-      </c>
-      <c r="K24" s="11">
-        <v>1355</v>
-      </c>
-      <c r="L24" s="12"/>
-      <c r="M24" s="13">
+        <v>1344</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1421</v>
+      </c>
+      <c r="I24" s="9">
+        <v>1351</v>
+      </c>
+      <c r="J24" s="9">
+        <v>1369</v>
+      </c>
+      <c r="K24" s="9">
+        <v>1190</v>
+      </c>
+      <c r="L24" s="9">
+        <v>1309</v>
+      </c>
+      <c r="M24" s="19">
         <f t="shared" si="0"/>
-        <v>1223</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="25" ht="15.75" spans="2:13">
@@ -2093,22 +2163,24 @@
         <v>2453</v>
       </c>
       <c r="G25" s="9">
-        <v>2505</v>
-      </c>
-      <c r="H25" s="9">
-        <v>2809</v>
-      </c>
-      <c r="I25" s="11">
-        <v>3454</v>
-      </c>
-      <c r="J25" s="11">
-        <v>3454</v>
-      </c>
-      <c r="K25" s="11">
-        <v>3454</v>
-      </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="13">
+        <v>2373</v>
+      </c>
+      <c r="H25" s="10">
+        <v>2829</v>
+      </c>
+      <c r="I25" s="9">
+        <v>2507</v>
+      </c>
+      <c r="J25" s="9">
+        <v>2721</v>
+      </c>
+      <c r="K25" s="9">
+        <v>2569</v>
+      </c>
+      <c r="L25" s="9">
+        <v>2345</v>
+      </c>
+      <c r="M25" s="19">
         <f t="shared" si="0"/>
         <v>2280</v>
       </c>
@@ -2130,22 +2202,24 @@
         <v>4336.48</v>
       </c>
       <c r="G26" s="9">
-        <v>5788.35</v>
-      </c>
-      <c r="H26" s="9">
-        <v>5366.16</v>
-      </c>
-      <c r="I26" s="11">
-        <v>4649.79</v>
-      </c>
-      <c r="J26" s="11">
-        <v>4649.79</v>
-      </c>
-      <c r="K26" s="11">
-        <v>4739.94</v>
-      </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="13">
+        <v>5265.86</v>
+      </c>
+      <c r="H26" s="10">
+        <v>4936.38</v>
+      </c>
+      <c r="I26" s="9">
+        <v>6180.69</v>
+      </c>
+      <c r="J26" s="9">
+        <v>4924.96</v>
+      </c>
+      <c r="K26" s="9">
+        <v>6760.85</v>
+      </c>
+      <c r="L26" s="9">
+        <v>4975.68</v>
+      </c>
+      <c r="M26" s="19">
         <f t="shared" si="0"/>
         <v>4336.48</v>
       </c>
@@ -2167,24 +2241,26 @@
         <v>6877.07</v>
       </c>
       <c r="G27" s="9">
-        <v>6252.18</v>
-      </c>
-      <c r="H27" s="9">
-        <v>6194.75</v>
-      </c>
-      <c r="I27" s="11">
-        <v>6400.64</v>
-      </c>
-      <c r="J27" s="11">
-        <v>6400.64</v>
-      </c>
-      <c r="K27" s="11">
-        <v>6400.64</v>
-      </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="13">
+        <v>6157.73</v>
+      </c>
+      <c r="H27" s="10">
+        <v>6664.7</v>
+      </c>
+      <c r="I27" s="9">
+        <v>6755.51</v>
+      </c>
+      <c r="J27" s="9">
+        <v>6823.53</v>
+      </c>
+      <c r="K27" s="9">
+        <v>7706.77</v>
+      </c>
+      <c r="L27" s="9">
+        <v>5185.34</v>
+      </c>
+      <c r="M27" s="19">
         <f t="shared" si="0"/>
-        <v>5798.54</v>
+        <v>5185.34</v>
       </c>
     </row>
     <row r="28" ht="15.75" spans="2:13">
@@ -2204,24 +2280,26 @@
         <v>8408.96</v>
       </c>
       <c r="G28" s="9">
-        <v>8544.86</v>
-      </c>
-      <c r="H28" s="9">
-        <v>8357.16</v>
-      </c>
-      <c r="I28" s="11">
-        <v>6767.07</v>
-      </c>
-      <c r="J28" s="11">
-        <v>6767.07</v>
-      </c>
-      <c r="K28" s="11">
-        <v>6767.07</v>
-      </c>
-      <c r="L28" s="12"/>
-      <c r="M28" s="13">
+        <v>8908.73</v>
+      </c>
+      <c r="H28" s="10">
+        <v>7861.19</v>
+      </c>
+      <c r="I28" s="9">
+        <v>8319.93</v>
+      </c>
+      <c r="J28" s="9">
+        <v>7498.89</v>
+      </c>
+      <c r="K28" s="9">
+        <v>9004.77</v>
+      </c>
+      <c r="L28" s="9">
+        <v>7754.96</v>
+      </c>
+      <c r="M28" s="19">
         <f t="shared" si="0"/>
-        <v>6767.07</v>
+        <v>7012.33</v>
       </c>
     </row>
     <row r="29" ht="15.75" spans="2:13">
@@ -2241,22 +2319,24 @@
         <v>5236.97</v>
       </c>
       <c r="G29" s="9">
-        <v>6080.13</v>
-      </c>
-      <c r="H29" s="9">
-        <v>5651.38</v>
-      </c>
-      <c r="I29" s="11">
-        <v>5393.56</v>
-      </c>
-      <c r="J29" s="11">
-        <v>5393.56</v>
-      </c>
-      <c r="K29" s="11">
-        <v>5393.56</v>
-      </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="13">
+        <v>4510.19</v>
+      </c>
+      <c r="H29" s="10">
+        <v>5005.16</v>
+      </c>
+      <c r="I29" s="9">
+        <v>5180.53</v>
+      </c>
+      <c r="J29" s="9">
+        <v>6071.02</v>
+      </c>
+      <c r="K29" s="9">
+        <v>5741.69</v>
+      </c>
+      <c r="L29" s="9">
+        <v>4572.51</v>
+      </c>
+      <c r="M29" s="19">
         <f t="shared" si="0"/>
         <v>4122.76</v>
       </c>
@@ -2278,24 +2358,26 @@
         <v>7329.84</v>
       </c>
       <c r="G30" s="9">
-        <v>6972.6</v>
-      </c>
-      <c r="H30" s="9">
-        <v>6092.16</v>
-      </c>
-      <c r="I30" s="11">
-        <v>5053.72</v>
-      </c>
-      <c r="J30" s="11">
-        <v>5053.72</v>
-      </c>
-      <c r="K30" s="11">
-        <v>5053.72</v>
-      </c>
-      <c r="L30" s="12"/>
-      <c r="M30" s="13">
+        <v>6976.99</v>
+      </c>
+      <c r="H30" s="10">
+        <v>7776.6</v>
+      </c>
+      <c r="I30" s="9">
+        <v>7683.59</v>
+      </c>
+      <c r="J30" s="9">
+        <v>6904.22</v>
+      </c>
+      <c r="K30" s="9">
+        <v>6986.52</v>
+      </c>
+      <c r="L30" s="9">
+        <v>8805.03</v>
+      </c>
+      <c r="M30" s="19">
         <f t="shared" si="0"/>
-        <v>5053.72</v>
+        <v>6904.22</v>
       </c>
     </row>
     <row r="31" ht="15.75" spans="2:13">
@@ -2315,24 +2397,26 @@
         <v>8493.57</v>
       </c>
       <c r="G31" s="9">
-        <v>8505.9</v>
-      </c>
-      <c r="H31" s="9">
-        <v>8469.14</v>
-      </c>
-      <c r="I31" s="11">
-        <v>6380.15</v>
-      </c>
-      <c r="J31" s="11">
-        <v>6486.19</v>
-      </c>
-      <c r="K31" s="11">
-        <v>6486.19</v>
-      </c>
-      <c r="L31" s="12"/>
-      <c r="M31" s="13">
+        <v>9109.66</v>
+      </c>
+      <c r="H31" s="10">
+        <v>8113.64</v>
+      </c>
+      <c r="I31" s="9">
+        <v>7256.23</v>
+      </c>
+      <c r="J31" s="9">
+        <v>9075.07</v>
+      </c>
+      <c r="K31" s="9">
+        <v>8530.14</v>
+      </c>
+      <c r="L31" s="9">
+        <v>7502.23</v>
+      </c>
+      <c r="M31" s="19">
         <f t="shared" si="0"/>
-        <v>6380.15</v>
+        <v>7256.23</v>
       </c>
     </row>
     <row r="32" ht="15.75" spans="2:13">
@@ -2352,24 +2436,26 @@
         <v>4986.24</v>
       </c>
       <c r="G32" s="9">
-        <v>6317.44</v>
-      </c>
-      <c r="H32" s="9">
-        <v>6075</v>
-      </c>
-      <c r="I32" s="11">
-        <v>4275.81</v>
-      </c>
-      <c r="J32" s="11">
-        <v>4275.81</v>
-      </c>
-      <c r="K32" s="11">
-        <v>4275.81</v>
-      </c>
-      <c r="L32" s="12"/>
-      <c r="M32" s="13">
+        <v>5239.95</v>
+      </c>
+      <c r="H32" s="10">
+        <v>4683.9</v>
+      </c>
+      <c r="I32" s="9">
+        <v>5590.49</v>
+      </c>
+      <c r="J32" s="9">
+        <v>5709.34</v>
+      </c>
+      <c r="K32" s="9">
+        <v>6602.02</v>
+      </c>
+      <c r="L32" s="9">
+        <v>6896.21</v>
+      </c>
+      <c r="M32" s="19">
         <f t="shared" si="0"/>
-        <v>4275.81</v>
+        <v>4683.9</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="2:13">
@@ -2389,22 +2475,24 @@
         <v>4425.8</v>
       </c>
       <c r="G33" s="9">
-        <v>6724.01</v>
-      </c>
-      <c r="H33" s="9">
-        <v>6515.93</v>
-      </c>
-      <c r="I33" s="11">
-        <v>5235.81</v>
-      </c>
-      <c r="J33" s="11">
-        <v>5235.81</v>
-      </c>
-      <c r="K33" s="11">
-        <v>5235.81</v>
-      </c>
-      <c r="L33" s="12"/>
-      <c r="M33" s="13">
+        <v>5472.22</v>
+      </c>
+      <c r="H33" s="10">
+        <v>5490.4</v>
+      </c>
+      <c r="I33" s="9">
+        <v>4875.19</v>
+      </c>
+      <c r="J33" s="9">
+        <v>5765.55</v>
+      </c>
+      <c r="K33" s="9">
+        <v>4657.96</v>
+      </c>
+      <c r="L33" s="9">
+        <v>4559.73</v>
+      </c>
+      <c r="M33" s="19">
         <f t="shared" si="0"/>
         <v>4425.8</v>
       </c>
@@ -2426,24 +2514,26 @@
         <v>3722.13</v>
       </c>
       <c r="G34" s="9">
-        <v>6193.36</v>
-      </c>
-      <c r="H34" s="9">
-        <v>7289.37</v>
-      </c>
-      <c r="I34" s="11">
-        <v>3894.47</v>
-      </c>
-      <c r="J34" s="11">
-        <v>3894.47</v>
-      </c>
-      <c r="K34" s="11">
-        <v>3894.47</v>
-      </c>
-      <c r="L34" s="12"/>
-      <c r="M34" s="13">
+        <v>3709.07</v>
+      </c>
+      <c r="H34" s="10">
+        <v>3726.62</v>
+      </c>
+      <c r="I34" s="9">
+        <v>4480.24</v>
+      </c>
+      <c r="J34" s="9">
+        <v>3709.07</v>
+      </c>
+      <c r="K34" s="9">
+        <v>5306.51</v>
+      </c>
+      <c r="L34" s="9">
+        <v>4957.66</v>
+      </c>
+      <c r="M34" s="19">
         <f t="shared" si="0"/>
-        <v>3722.13</v>
+        <v>3709.07</v>
       </c>
     </row>
     <row r="35" ht="15.75" spans="2:13">
@@ -2463,24 +2553,26 @@
         <v>3034.12</v>
       </c>
       <c r="G35" s="9">
-        <v>3835.25</v>
-      </c>
-      <c r="H35" s="9">
-        <v>3899.52</v>
-      </c>
-      <c r="I35" s="11">
-        <v>2043.71</v>
-      </c>
-      <c r="J35" s="11">
-        <v>2043.71</v>
-      </c>
-      <c r="K35" s="11">
-        <v>2043.71</v>
-      </c>
-      <c r="L35" s="12"/>
-      <c r="M35" s="13">
+        <v>3304.31</v>
+      </c>
+      <c r="H35" s="10">
+        <v>3186.42</v>
+      </c>
+      <c r="I35" s="9">
+        <v>3158.03</v>
+      </c>
+      <c r="J35" s="9">
+        <v>3543.73</v>
+      </c>
+      <c r="K35" s="9">
+        <v>3500.09</v>
+      </c>
+      <c r="L35" s="9">
+        <v>3182.16</v>
+      </c>
+      <c r="M35" s="19">
         <f>SMALL(D35:L35,1)</f>
-        <v>2043.71</v>
+        <v>2666.73</v>
       </c>
     </row>
     <row r="36" ht="15.75" spans="2:13">
@@ -2500,22 +2592,24 @@
         <v>18820.19</v>
       </c>
       <c r="G36" s="9">
-        <v>23849.18</v>
-      </c>
-      <c r="H36" s="9">
-        <v>27345.87</v>
-      </c>
-      <c r="I36" s="11">
-        <v>21502.18</v>
-      </c>
-      <c r="J36" s="11">
-        <v>21502.18</v>
-      </c>
-      <c r="K36" s="11">
-        <v>21502.18</v>
-      </c>
-      <c r="L36" s="12"/>
-      <c r="M36" s="13">
+        <v>21635.4</v>
+      </c>
+      <c r="H36" s="10">
+        <v>19279.1</v>
+      </c>
+      <c r="I36" s="9">
+        <v>21573.3</v>
+      </c>
+      <c r="J36" s="9">
+        <v>21234.24</v>
+      </c>
+      <c r="K36" s="9">
+        <v>23034.81</v>
+      </c>
+      <c r="L36" s="9">
+        <v>22639.34</v>
+      </c>
+      <c r="M36" s="19">
         <f>SMALL(D36:L36,1)</f>
         <v>18820.19</v>
       </c>
@@ -2537,22 +2631,24 @@
         <v>14206.16</v>
       </c>
       <c r="G37" s="9">
-        <v>15392.18</v>
-      </c>
-      <c r="H37" s="9">
-        <v>20046.48</v>
-      </c>
-      <c r="I37" s="11">
-        <v>7221.99</v>
-      </c>
-      <c r="J37" s="11">
-        <v>7221.99</v>
-      </c>
-      <c r="K37" s="11">
-        <v>7221.99</v>
-      </c>
-      <c r="L37" s="12"/>
-      <c r="M37" s="13">
+        <v>6733.38</v>
+      </c>
+      <c r="H37" s="10">
+        <v>17694.99</v>
+      </c>
+      <c r="I37" s="9">
+        <v>14689.12</v>
+      </c>
+      <c r="J37" s="9">
+        <v>17573.58</v>
+      </c>
+      <c r="K37" s="9">
+        <v>14588.58</v>
+      </c>
+      <c r="L37" s="9">
+        <v>15763.57</v>
+      </c>
+      <c r="M37" s="19">
         <f>SMALL(D37:L37,1)</f>
         <v>6733.38</v>
       </c>
@@ -2574,22 +2670,24 @@
         <v>16746.21</v>
       </c>
       <c r="G38" s="9">
-        <v>18071.56</v>
-      </c>
-      <c r="H38" s="9">
-        <v>18269.04</v>
-      </c>
-      <c r="I38" s="11">
-        <v>10080.05</v>
-      </c>
-      <c r="J38" s="11">
-        <v>10080.05</v>
-      </c>
-      <c r="K38" s="11">
-        <v>10080.05</v>
-      </c>
-      <c r="L38" s="12"/>
-      <c r="M38" s="13">
+        <v>9284.41</v>
+      </c>
+      <c r="H38" s="10">
+        <v>17598.69</v>
+      </c>
+      <c r="I38" s="9">
+        <v>23034.35</v>
+      </c>
+      <c r="J38" s="9">
+        <v>10953.62</v>
+      </c>
+      <c r="K38" s="9">
+        <v>9589.94</v>
+      </c>
+      <c r="L38" s="9">
+        <v>9378.8</v>
+      </c>
+      <c r="M38" s="19">
         <f>SMALL(D38:L38,1)</f>
         <v>9284.41</v>
       </c>
@@ -2611,24 +2709,26 @@
         <v>26536.33</v>
       </c>
       <c r="G39" s="9">
-        <v>28584.18</v>
-      </c>
-      <c r="H39" s="9">
-        <v>27441.89</v>
-      </c>
-      <c r="I39" s="11">
-        <v>20714.89</v>
-      </c>
-      <c r="J39" s="11">
-        <v>20642.54</v>
-      </c>
-      <c r="K39" s="11">
-        <v>20642.54</v>
-      </c>
-      <c r="L39" s="12"/>
-      <c r="M39" s="13">
+        <v>25812.1</v>
+      </c>
+      <c r="H39" s="10">
+        <v>24766.15</v>
+      </c>
+      <c r="I39" s="9">
+        <v>24457.55</v>
+      </c>
+      <c r="J39" s="9">
+        <v>25049.58</v>
+      </c>
+      <c r="K39" s="9">
+        <v>24701.38</v>
+      </c>
+      <c r="L39" s="9">
+        <v>32130.8</v>
+      </c>
+      <c r="M39" s="19">
         <f>SMALL(D39:L39,1)</f>
-        <v>20642.54</v>
+        <v>23765.41</v>
       </c>
     </row>
     <row r="40" ht="15.75" spans="2:13">
@@ -2648,24 +2748,26 @@
         <v>15889.78</v>
       </c>
       <c r="G40" s="9">
-        <v>21665.33</v>
-      </c>
-      <c r="H40" s="9">
-        <v>21566.81</v>
-      </c>
-      <c r="I40" s="11">
-        <v>10742.86</v>
-      </c>
-      <c r="J40" s="11">
-        <v>10742.86</v>
-      </c>
-      <c r="K40" s="11">
-        <v>10742.86</v>
-      </c>
-      <c r="L40" s="12"/>
-      <c r="M40" s="13">
+        <v>18860.85</v>
+      </c>
+      <c r="H40" s="10">
+        <v>23986.36</v>
+      </c>
+      <c r="I40" s="9">
+        <v>22683.91</v>
+      </c>
+      <c r="J40" s="9">
+        <v>19733.38</v>
+      </c>
+      <c r="K40" s="9">
+        <v>16412.75</v>
+      </c>
+      <c r="L40" s="9">
+        <v>17142.83</v>
+      </c>
+      <c r="M40" s="19">
         <f>SMALL(D40:L40,1)</f>
-        <v>10742.86</v>
+        <v>15000.67</v>
       </c>
     </row>
     <row r="41" ht="15.75" spans="2:13">
@@ -2685,24 +2787,26 @@
         <v>24984.11</v>
       </c>
       <c r="G41" s="9">
-        <v>22847.04</v>
-      </c>
-      <c r="H41" s="9">
-        <v>27196.36</v>
-      </c>
-      <c r="I41" s="11">
-        <v>14780.62</v>
-      </c>
-      <c r="J41" s="11">
-        <v>14780.62</v>
-      </c>
-      <c r="K41" s="11">
-        <v>14780.62</v>
-      </c>
-      <c r="L41" s="12"/>
-      <c r="M41" s="13">
+        <v>26763.92</v>
+      </c>
+      <c r="H41" s="10">
+        <v>27601.57</v>
+      </c>
+      <c r="I41" s="9">
+        <v>23216.28</v>
+      </c>
+      <c r="J41" s="9">
+        <v>24512.04</v>
+      </c>
+      <c r="K41" s="9">
+        <v>25117.47</v>
+      </c>
+      <c r="L41" s="9">
+        <v>25715.23</v>
+      </c>
+      <c r="M41" s="19">
         <f>SMALL(D41:L41,1)</f>
-        <v>14780.62</v>
+        <v>20797.27</v>
       </c>
     </row>
     <row r="42" ht="15.75" spans="2:13">
@@ -2722,24 +2826,26 @@
         <v>296.91</v>
       </c>
       <c r="G42" s="9">
-        <v>298.55</v>
-      </c>
-      <c r="H42" s="9">
-        <v>290.63</v>
-      </c>
-      <c r="I42" s="11">
-        <v>255.03</v>
-      </c>
-      <c r="J42" s="11">
-        <v>255.03</v>
-      </c>
-      <c r="K42" s="11">
-        <v>255.03</v>
-      </c>
-      <c r="L42" s="12"/>
-      <c r="M42" s="13">
+        <v>272.54</v>
+      </c>
+      <c r="H42" s="10">
+        <v>256.31</v>
+      </c>
+      <c r="I42" s="9">
+        <v>318.19</v>
+      </c>
+      <c r="J42" s="9">
+        <v>302.39</v>
+      </c>
+      <c r="K42" s="9">
+        <v>268.54</v>
+      </c>
+      <c r="L42" s="9">
+        <v>291.1</v>
+      </c>
+      <c r="M42" s="19">
         <f>SMALL(D42:L42,1)</f>
-        <v>255.03</v>
+        <v>256.31</v>
       </c>
     </row>
     <row r="43" ht="15.75" spans="2:13">
@@ -2759,22 +2865,24 @@
         <v>545.52</v>
       </c>
       <c r="G43" s="9">
-        <v>694.29</v>
-      </c>
-      <c r="H43" s="9">
-        <v>700.1</v>
-      </c>
-      <c r="I43" s="11">
-        <v>529.26</v>
-      </c>
-      <c r="J43" s="11">
-        <v>529.26</v>
-      </c>
-      <c r="K43" s="11">
-        <v>529.26</v>
-      </c>
-      <c r="L43" s="12"/>
-      <c r="M43" s="13">
+        <v>556.73</v>
+      </c>
+      <c r="H43" s="10">
+        <v>546.02</v>
+      </c>
+      <c r="I43" s="9">
+        <v>580.47</v>
+      </c>
+      <c r="J43" s="9">
+        <v>554.79</v>
+      </c>
+      <c r="K43" s="9">
+        <v>540.73</v>
+      </c>
+      <c r="L43" s="9">
+        <v>571.34</v>
+      </c>
+      <c r="M43" s="19">
         <f>SMALL(D43:L43,1)</f>
         <v>523.7</v>
       </c>
@@ -2796,24 +2904,26 @@
         <v>4864</v>
       </c>
       <c r="G44" s="9">
-        <v>5056</v>
-      </c>
-      <c r="H44" s="9">
-        <v>5093</v>
-      </c>
-      <c r="I44" s="11">
-        <v>5015</v>
-      </c>
-      <c r="J44" s="11">
-        <v>5015</v>
-      </c>
-      <c r="K44" s="11">
-        <v>5015</v>
-      </c>
-      <c r="L44" s="12"/>
-      <c r="M44" s="13">
+        <v>4763</v>
+      </c>
+      <c r="H44" s="10">
+        <v>4786</v>
+      </c>
+      <c r="I44" s="9">
+        <v>4703</v>
+      </c>
+      <c r="J44" s="9">
+        <v>4850</v>
+      </c>
+      <c r="K44" s="9">
+        <v>5047</v>
+      </c>
+      <c r="L44" s="9">
+        <v>4709</v>
+      </c>
+      <c r="M44" s="19">
         <f>SMALL(D44:L44,1)</f>
-        <v>4782</v>
+        <v>4703</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="2:13">
@@ -2833,24 +2943,26 @@
         <v>122.13</v>
       </c>
       <c r="G45" s="9">
-        <v>161.9</v>
-      </c>
-      <c r="H45" s="9">
-        <v>173.28</v>
-      </c>
-      <c r="I45" s="11">
-        <v>129.15</v>
-      </c>
-      <c r="J45" s="11">
-        <v>129.15</v>
-      </c>
-      <c r="K45" s="11">
-        <v>129.15</v>
-      </c>
-      <c r="L45" s="12"/>
-      <c r="M45" s="13">
+        <v>123.01</v>
+      </c>
+      <c r="H45" s="10">
+        <v>136.12</v>
+      </c>
+      <c r="I45" s="9">
+        <v>117.21</v>
+      </c>
+      <c r="J45" s="9">
+        <v>127.64</v>
+      </c>
+      <c r="K45" s="9">
+        <v>127.34</v>
+      </c>
+      <c r="L45" s="9">
+        <v>118.93</v>
+      </c>
+      <c r="M45" s="19">
         <f>SMALL(D45:L45,1)</f>
-        <v>117.32</v>
+        <v>117.21</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="2:13">
@@ -2870,24 +2982,26 @@
         <v>152</v>
       </c>
       <c r="G46" s="9">
-        <v>146</v>
-      </c>
-      <c r="H46" s="9">
-        <v>146</v>
-      </c>
-      <c r="I46" s="11">
-        <v>146</v>
-      </c>
-      <c r="J46" s="11">
-        <v>146</v>
-      </c>
-      <c r="K46" s="11">
-        <v>146</v>
-      </c>
-      <c r="L46" s="12"/>
-      <c r="M46" s="13">
+        <v>150</v>
+      </c>
+      <c r="H46" s="10">
+        <v>150</v>
+      </c>
+      <c r="I46" s="9">
+        <v>173</v>
+      </c>
+      <c r="J46" s="9">
+        <v>174</v>
+      </c>
+      <c r="K46" s="9">
+        <v>150</v>
+      </c>
+      <c r="L46" s="9">
+        <v>172</v>
+      </c>
+      <c r="M46" s="19">
         <f>SMALL(D46:L46,1)</f>
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" ht="15.75" spans="2:13">
@@ -2907,22 +3021,24 @@
         <v>638.03</v>
       </c>
       <c r="G47" s="9">
-        <v>714.33</v>
-      </c>
-      <c r="H47" s="9">
-        <v>714.33</v>
-      </c>
-      <c r="I47" s="11">
+        <v>751.06</v>
+      </c>
+      <c r="H47" s="10">
         <v>638.03</v>
       </c>
-      <c r="J47" s="11">
+      <c r="I47" s="9">
+        <v>751.06</v>
+      </c>
+      <c r="J47" s="9">
+        <v>751.06</v>
+      </c>
+      <c r="K47" s="9">
         <v>638.03</v>
       </c>
-      <c r="K47" s="11">
+      <c r="L47" s="9">
         <v>638.03</v>
       </c>
-      <c r="L47" s="12"/>
-      <c r="M47" s="13">
+      <c r="M47" s="19">
         <f>SMALL(D47:L47,1)</f>
         <v>638.03</v>
       </c>
@@ -2944,62 +3060,134 @@
         <v>904.31</v>
       </c>
       <c r="G48" s="9">
-        <v>1222.15</v>
-      </c>
-      <c r="H48" s="9">
-        <v>931.78</v>
-      </c>
-      <c r="I48" s="11">
+        <v>755.79</v>
+      </c>
+      <c r="H48" s="10">
+        <v>790.01</v>
+      </c>
+      <c r="I48" s="9">
         <v>456.58</v>
       </c>
-      <c r="J48" s="11">
+      <c r="J48" s="9">
         <v>456.58</v>
       </c>
-      <c r="K48" s="11">
-        <v>456.58</v>
-      </c>
-      <c r="L48" s="12"/>
-      <c r="M48" s="13">
+      <c r="K48" s="9">
+        <v>755.79</v>
+      </c>
+      <c r="L48" s="9">
+        <v>755.79</v>
+      </c>
+      <c r="M48" s="19">
         <f>SMALL(D48:L48,1)</f>
         <v>456.58</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
-      <c r="B49">
-        <v>44</v>
-      </c>
-      <c r="D49">
+    <row r="49" spans="2:12">
+      <c r="B49" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13">
+        <v>13</v>
+      </c>
+      <c r="E49" s="13">
+        <v>13</v>
+      </c>
+      <c r="F49" s="13">
+        <v>10</v>
+      </c>
+      <c r="G49" s="13">
+        <v>12</v>
+      </c>
+      <c r="H49" s="13">
         <v>7</v>
       </c>
-      <c r="E49">
-        <v>5</v>
-      </c>
-      <c r="F49">
-        <v>45</v>
-      </c>
-      <c r="G49">
-        <v>48</v>
-      </c>
-      <c r="H49">
-        <v>42</v>
-      </c>
-      <c r="I49">
-        <v>43</v>
-      </c>
-      <c r="J49">
-        <v>49</v>
-      </c>
-      <c r="K49">
-        <v>44</v>
+      <c r="I49" s="13">
+        <v>11</v>
+      </c>
+      <c r="J49" s="13">
+        <v>8</v>
+      </c>
+      <c r="K49" s="13">
+        <v>11</v>
+      </c>
+      <c r="L49" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" ht="20" customHeight="1" spans="2:12">
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+    </row>
+    <row r="51" ht="15.75" spans="2:12">
+      <c r="B51" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="16">
+        <f>AVERAGE(D5:D48)</f>
+        <v>5119.59727272727</v>
+      </c>
+      <c r="E51" s="17">
+        <f>AVERAGE(E5:E48)</f>
+        <v>4770.76772727273</v>
+      </c>
+      <c r="F51" s="17">
+        <f>AVERAGE(F5:F48)</f>
+        <v>5118.365</v>
+      </c>
+      <c r="G51" s="17">
+        <f t="shared" ref="E51:L51" si="1">AVERAGE(G5:G48)</f>
+        <v>4954.20477272727</v>
+      </c>
+      <c r="H51" s="16">
+        <f t="shared" si="1"/>
+        <v>5552.23272727273</v>
+      </c>
+      <c r="I51" s="16">
+        <f t="shared" si="1"/>
+        <v>5535.04590909091</v>
+      </c>
+      <c r="J51" s="16">
+        <f t="shared" si="1"/>
+        <v>5167.36340909091</v>
+      </c>
+      <c r="K51" s="16">
+        <f t="shared" si="1"/>
+        <v>5271.93659090909</v>
+      </c>
+      <c r="L51" s="16">
+        <f t="shared" si="1"/>
+        <v>5371.26772727273</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="16">
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="D3:L3"/>
+    <mergeCell ref="B51:C51"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="K49:K50"/>
+    <mergeCell ref="L49:L50"/>
     <mergeCell ref="M3:M4"/>
+    <mergeCell ref="B49:C50"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:L5">
     <cfRule type="cellIs" dxfId="0" priority="53" operator="equal">

</xml_diff>